<commit_message>
Updated the instructions and rubric
</commit_message>
<xml_diff>
--- a/LabStarters/Lab07/Lab7Rubric-CIS195.xlsx
+++ b/LabStarters/Lab07/Lab7Rubric-CIS195.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CIS195-CourseMaterials/LabStarters/Lab07/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/LabStarters/Lab07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D2D02C-E9C6-7743-B4D8-0B1F349AB997}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C35C5D74-77EF-0648-A6C6-923FF74DA5B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="460" windowWidth="18120" windowHeight="17000" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="3320" yWindow="500" windowWidth="18120" windowHeight="16520" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Requirements:</t>
   </si>
@@ -43,12 +43,6 @@
     <t>Subtotal</t>
   </si>
   <si>
-    <t>Part 1: Raffle contest form</t>
-  </si>
-  <si>
-    <t>Part 2: TBD</t>
-  </si>
-  <si>
     <t>We only did part 1 for fall term, 2019</t>
   </si>
   <si>
@@ -85,22 +79,19 @@
     <t>Set background color for fields (a different color)</t>
   </si>
   <si>
-    <t>For next term:</t>
-  </si>
-  <si>
-    <t>Make a new part 1 that is easier</t>
-  </si>
-  <si>
-    <t>Use this term's part 1 as part 2</t>
-  </si>
-  <si>
-    <t>Lab 7, Tables</t>
-  </si>
-  <si>
     <t>heading (like &lt;h1&gt;) in header for page</t>
   </si>
   <si>
     <t>Syntax and style</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Forms</t>
+  </si>
+  <si>
+    <t>Raffle contest form</t>
   </si>
 </sst>
 </file>
@@ -172,7 +163,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -180,11 +171,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -199,6 +199,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,289 +516,163 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7896AEF-34AA-E746-914C-B3A1A695E7D1}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="1" max="1" width="44" customWidth="1"/>
+    <col min="2" max="2" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>7</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>5</v>
-      </c>
-      <c r="F9">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="E10">
-        <v>8</v>
-      </c>
-      <c r="F10">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="4">
-        <v>4</v>
-      </c>
-      <c r="C11" s="4">
-        <v>4</v>
-      </c>
-      <c r="E11" s="4">
-        <v>7</v>
-      </c>
-      <c r="F11" s="4">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C11"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B12" s="4">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="E14">
-        <v>4</v>
-      </c>
-      <c r="F14">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="E15">
-        <v>4</v>
-      </c>
-      <c r="F15">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
-      </c>
-      <c r="F16">
+        <v>18</v>
+      </c>
+      <c r="B16" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="3">
         <f>SUM(B4:B16)</f>
-        <v>30</v>
-      </c>
-      <c r="C17" s="3">
-        <f>SUM(C4:C16)</f>
-        <v>30</v>
-      </c>
-      <c r="E17" s="3">
-        <f>SUM(E4:E16)</f>
-        <v>50</v>
-      </c>
-      <c r="F17" s="3">
-        <f>SUM(F4:F16)</f>
-        <v>50</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E19" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>21</v>
-      </c>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
@@ -810,30 +685,14 @@
       <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="3">
-        <f>SUM(B22:B23)</f>
-        <v>0</v>
-      </c>
-      <c r="C24" s="3">
-        <f>SUM(C22:C23)</f>
-        <v>0</v>
-      </c>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="5">
-        <f>SUM(B17,B24)</f>
-        <v>30</v>
-      </c>
-      <c r="C25" s="5">
-        <f>SUM(C17,C24)</f>
-        <v>30</v>
-      </c>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -844,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="156" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -855,7 +714,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -871,7 +730,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -882,12 +741,12 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -898,7 +757,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -909,7 +768,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -920,7 +779,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -931,7 +790,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -942,7 +801,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="4">
         <v>7</v>
@@ -953,7 +812,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -964,12 +823,12 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -980,7 +839,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -991,7 +850,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>3</v>

</xml_diff>

<commit_message>
Improvements and bug fixes to auto grader, added requirements for lab 8
</commit_message>
<xml_diff>
--- a/LabStarters/Lab07/Lab7Rubric-CIS195.xlsx
+++ b/LabStarters/Lab07/Lab7Rubric-CIS195.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/LabStarters/Lab07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C35C5D74-77EF-0648-A6C6-923FF74DA5B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530147E3-E519-554F-80E6-8C99A574479A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="500" windowWidth="18120" windowHeight="16520" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="9800" yWindow="500" windowWidth="18120" windowHeight="16520" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>Requirements:</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Subtotal</t>
   </si>
   <si>
-    <t>We only did part 1 for fall term, 2019</t>
-  </si>
-  <si>
     <t>Form input elements:</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>Labels for all input elements</t>
   </si>
   <si>
-    <t>Form footer</t>
-  </si>
-  <si>
     <t>Embedded CSS</t>
   </si>
   <si>
@@ -92,6 +86,21 @@
   </si>
   <si>
     <t>Raffle contest form</t>
+  </si>
+  <si>
+    <t>We have only done part 1 since fall term, 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set background color for fields </t>
+  </si>
+  <si>
+    <t>Page footer</t>
+  </si>
+  <si>
+    <t>Published to a web server</t>
+  </si>
+  <si>
+    <t>tel not used</t>
   </si>
 </sst>
 </file>
@@ -184,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -199,7 +208,8 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7896AEF-34AA-E746-914C-B3A1A695E7D1}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,12 +538,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="8"/>
     </row>
@@ -542,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2"/>
       <c r="E3" s="2"/>
@@ -550,7 +560,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -558,28 +568,28 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -587,7 +597,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -595,7 +605,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -603,7 +613,7 @@
     </row>
     <row r="11" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="4">
         <v>5</v>
@@ -612,21 +622,21 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -634,7 +644,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -642,42 +652,45 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="3">
-        <f>SUM(B4:B16)</f>
+      <c r="A17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3">
+        <f>SUM(B4:B17)</f>
         <v>40</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E19" s="8"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="E21" s="9"/>
+      <c r="A21" s="1"/>
+      <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
@@ -685,14 +698,19 @@
       <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -701,23 +719,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView zoomScale="156" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" customWidth="1"/>
+    <col min="4" max="4" width="1.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -728,167 +745,183 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="C9">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C10" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4">
-        <v>7</v>
-      </c>
-      <c r="C10" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>15</v>
-      </c>
       <c r="B13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="3">
-        <f>SUM(B3:B15)</f>
-        <v>50</v>
-      </c>
-      <c r="C16" s="3">
-        <f>SUM(C3:C15)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B15" s="10">
+        <v>3</v>
+      </c>
+      <c r="C15" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="11">
+        <v>4</v>
+      </c>
+      <c r="C16" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3">
+        <f>SUM(B3:B16)</f>
+        <v>40</v>
+      </c>
+      <c r="C17" s="3">
+        <f>SUM(C3:C16)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More requirements csv files and  other updates
</commit_message>
<xml_diff>
--- a/LabStarters/Lab07/Lab7Rubric-CIS195.xlsx
+++ b/LabStarters/Lab07/Lab7Rubric-CIS195.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/LabStarters/Lab07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530147E3-E519-554F-80E6-8C99A574479A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611BCCF9-E6AA-454C-AAC3-6195C1FC406D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9800" yWindow="500" windowWidth="18120" windowHeight="16520" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Requirements:</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>Published to a web server</t>
-  </si>
-  <si>
-    <t>tel not used</t>
   </si>
 </sst>
 </file>
@@ -719,10 +716,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
-  <dimension ref="A2:E23"/>
+  <dimension ref="A2:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,7 +731,7 @@
     <col min="5" max="5" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -745,7 +742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -756,12 +753,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -772,7 +769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -783,7 +780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
@@ -791,13 +788,10 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -808,7 +802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -819,7 +813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -830,7 +824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -841,12 +835,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
@@ -857,7 +851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>21</v>
       </c>
@@ -868,7 +862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
@@ -879,7 +873,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>23</v>
       </c>
@@ -900,7 +894,7 @@
       </c>
       <c r="C17" s="3">
         <f>SUM(C3:C16)</f>
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>